<commit_message>
feat: add heat wave duration variable and update related translations and styles
</commit_message>
<xml_diff>
--- a/backend/data/climatologias_HW.xlsx
+++ b/backend/data/climatologias_HW.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hw_int" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="hw_dur" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t xml:space="preserve">Historical</t>
   </si>
@@ -80,8 +81,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -148,12 +150,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,8 +354,8 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="A1:H14 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,4 +720,380 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>4.19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>4.14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>4.14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>4.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>